<commit_message>
Added notes on NVMe logs
</commit_message>
<xml_diff>
--- a/docs/NVMe Log Pages Explained/nvme_log_pages.xlsx
+++ b/docs/NVMe Log Pages Explained/nvme_log_pages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Documents\grantcurell.github.io\docs\NVMe Log Pages Explained\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFFAB6B-59E2-423D-896F-03DCA1104B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DA0D4F1-B492-421E-BA83-8CD111FABDC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19330" yWindow="9180" windowWidth="19070" windowHeight="11820" xr2:uid="{660E0BDD-A99A-4C2D-BCAE-89D8303B978D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="79">
   <si>
     <t>Log</t>
   </si>
@@ -122,24 +122,15 @@
     <t>09h</t>
   </si>
   <si>
-    <t>endgidmax (endurance groups) is 0</t>
-  </si>
-  <si>
     <t>Predictable Latncy Per NVM Set</t>
   </si>
   <si>
-    <t xml:space="preserve">The drives only support one </t>
-  </si>
-  <si>
     <t>Predictable Latncy Event Aggregate Log Page</t>
   </si>
   <si>
     <t>Asymmetric Namespace Access</t>
   </si>
   <si>
-    <t>There is only one namespace</t>
-  </si>
-  <si>
     <t>FOR-AUSTIN</t>
   </si>
   <si>
@@ -158,9 +149,6 @@
     <t>Endurance Group Event Aggregate</t>
   </si>
   <si>
-    <t>Endurance groups not in use</t>
-  </si>
-  <si>
     <t>Media Unit Status</t>
   </si>
   <si>
@@ -182,31 +170,123 @@
     <t>10h</t>
   </si>
   <si>
-    <t>Used for NVM sets (not in use)</t>
-  </si>
-  <si>
     <t>Supported Capacity Configuration List</t>
   </si>
   <si>
     <t>11h</t>
   </si>
   <si>
-    <t>Used for defining configuration of endurance groups</t>
-  </si>
-  <si>
     <t>Feature Identifiers Supported and Effects</t>
   </si>
   <si>
     <t>12h</t>
+  </si>
+  <si>
+    <t>This command is not currently supported because there is only one endurance group (endgidmax=0)</t>
+  </si>
+  <si>
+    <t>This log is not supported because the drives only support one NVM Set.</t>
+  </si>
+  <si>
+    <t>This log is not supported because there is only one namespace on the drive.</t>
+  </si>
+  <si>
+    <t>This is not supported because endurance groups are not in use.</t>
+  </si>
+  <si>
+    <t>This page is not supported because it is used for NVM sets which are not in use.</t>
+  </si>
+  <si>
+    <t>This log page is not available because the drives do not currently support multiple endurance groups.</t>
+  </si>
+  <si>
+    <t>AUSTIN HELP - Do we maybe only have one instance of each of those interfaces or something?</t>
+  </si>
+  <si>
+    <t>NVMe-MI Commands Supported and Effects</t>
+  </si>
+  <si>
+    <t>13h</t>
+  </si>
+  <si>
+    <t>Maybe?</t>
+  </si>
+  <si>
+    <t>AUSTIN HELP - seems like it could be helpful? I haven't read through the management command spec though</t>
+  </si>
+  <si>
+    <t>Command and Feature Lockdown</t>
+  </si>
+  <si>
+    <t>14h</t>
+  </si>
+  <si>
+    <t>This command is not supported. It is used for preventing certain commands for security purposes. It is not relevant to performance testing.</t>
+  </si>
+  <si>
+    <t>Boot Partition</t>
+  </si>
+  <si>
+    <t>15h</t>
+  </si>
+  <si>
+    <t>This command is not supported and does not have any relevance to drive performance. It allows you to see the boot partition of the drive.</t>
+  </si>
+  <si>
+    <t>Rotational Media Information Log</t>
+  </si>
+  <si>
+    <t>16h</t>
+  </si>
+  <si>
+    <t>This is specific to multiple endurance groups so it is not supported (since there is only one)</t>
+  </si>
+  <si>
+    <t>Discovery Log Page</t>
+  </si>
+  <si>
+    <t>70h</t>
+  </si>
+  <si>
+    <t>This log page is not supported. It is specific to NVMe-over-Fabrics (ex: RDMA)</t>
+  </si>
+  <si>
+    <t>Reservation Notification</t>
+  </si>
+  <si>
+    <t>Probably Not</t>
+  </si>
+  <si>
+    <t>80h</t>
+  </si>
+  <si>
+    <t>AUSTIN HELP (I'm not familiar with reservation notifications)</t>
+  </si>
+  <si>
+    <t>Sanitize Status</t>
+  </si>
+  <si>
+    <t>81h</t>
+  </si>
+  <si>
+    <t>AUSTIN HELP - This one seems like it could be useful but I assume we don't implement the sanitize command or something?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -234,9 +314,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -553,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991F2DAD-C624-48D7-946B-E2B6ACD83E29}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5"/>
@@ -567,20 +650,20 @@
     <col min="6" max="16384" width="8.7265625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5" ht="23.5">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -675,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -709,7 +792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="29">
+    <row r="10" spans="1:5" ht="72.5">
       <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
@@ -723,143 +806,273 @@
         <v>11</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43.5">
+      <c r="A11" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="29">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="43.5">
+      <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="58">
+      <c r="A13" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="29">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="29">
-      <c r="A13" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="29">
       <c r="A14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="43.5">
+      <c r="A15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="58">
+      <c r="A16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="72.5">
+      <c r="A17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="29">
-      <c r="A15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="D17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="72.5">
+      <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="29">
-      <c r="A16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="43.5">
-      <c r="A17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="29">
-      <c r="A18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="D18" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="72.5">
+      <c r="A19" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="101.5">
+      <c r="A20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="101.5">
+      <c r="A21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="72.5">
+      <c r="A22" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="58">
+      <c r="A23" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="43.5">
+      <c r="A24" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="87">
+      <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>